<commit_message>
Added email notification when bulk creating users
</commit_message>
<xml_diff>
--- a/app/templates/sample_upload.xlsx
+++ b/app/templates/sample_upload.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kurt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kurt\Desktop\Projects\capstone_directory_api\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE712600-ADBD-4E44-BE51-39E35EEC2D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293907C8-C3AE-4D8A-8A49-7EAF323D3F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EFE41418-CCA7-4C54-A045-90A311246FB0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>First Name</t>
   </si>
@@ -78,36 +78,6 @@
   </si>
   <si>
     <t>Student</t>
-  </si>
-  <si>
-    <t>Administrator</t>
-  </si>
-  <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>Dimacali</t>
-  </si>
-  <si>
-    <t>2023-098765</t>
-  </si>
-  <si>
-    <t>joserovicdimacali@gmail.com</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>Game Developer</t>
-  </si>
-  <si>
-    <t>Terrence</t>
-  </si>
-  <si>
-    <t>Maculanlan</t>
-  </si>
-  <si>
-    <t>romeoterrencemaculanlan@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -663,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33EBF0D8-8A7D-430B-8D62-F8769C18802F}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,50 +700,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{79C8B3A5-D6E0-4C45-8110-E2D75AD0ABE1}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{0D3B334A-E9AC-49AA-8B8D-063126CB128C}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{9EA1DADE-1820-4C34-A5CD-A9058F877C53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>